<commit_message>
update to resProp and new conflictCat notebook
</commit_message>
<xml_diff>
--- a/war_index.xlsx
+++ b/war_index.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Desktop\PhD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\PhD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B5A492-EFF4-4887-9CDA-34BF58DA2DC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6683212F-28F3-4354-8602-DC7FAAB66422}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{04375B46-837D-49F2-BE8A-ABE006783F6C}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="55">
   <si>
     <t>date</t>
   </si>
@@ -173,6 +173,24 @@
   </si>
   <si>
     <t>Ludwig Yorck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">French Revolutionary Wars </t>
+  </si>
+  <si>
+    <t>Italian campaigns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">French Revolutionary Army </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Coalition of Austria, Russia, Piedmont-Sardinia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">First Coalition </t>
+  </si>
+  <si>
+    <t>1792–1797</t>
   </si>
 </sst>
 </file>
@@ -215,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -224,6 +242,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -541,20 +562,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C1708F5-F567-4565-A221-ECE07B210A7F}">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L17:L18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="20.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
@@ -589,16 +610,16 @@
       <c r="H1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4" t="s">
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
       <c r="P1" s="1" t="s">
         <v>18</v>
       </c>
@@ -779,60 +800,91 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+    </row>
+    <row r="14" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>19</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I14" s="1">
         <v>20000</v>
       </c>
-      <c r="L13" s="1">
+      <c r="L14" s="1">
         <v>2000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="G14" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="I14" s="1">
-        <v>18000</v>
-      </c>
-      <c r="L14" s="1">
-        <v>2800</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I15" s="1">
+        <v>18000</v>
+      </c>
+      <c r="L15" s="1">
+        <v>2800</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I16" s="1">
         <v>9000</v>
       </c>
-      <c r="L15" s="1">
+      <c r="L16" s="1">
         <v>900</v>
       </c>
     </row>

</xml_diff>